<commit_message>
Developed the test methods and prepared the test scripts and test data for Customer features
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/AutmationBlockers.xlsx
+++ b/Mobile/coyni_mobile/resources/AutmationBlockers.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_V3.0_Personal\19-July-2023_v3.0\coyni-automation\Mobile\coyni_mobile\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ideyalabs/Documents/24-July-2023_v3.0_Android/coyni-automation/Mobile/coyni_mobile/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9D7A98-3981-42DF-BC04-56976E819DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5D5C4E-9E73-044C-8ED2-ACE994E7AC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6789F843-B6C6-469F-91AB-D7541C9DA822}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{6789F843-B6C6-469F-91AB-D7541C9DA822}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blockers" sheetId="1" r:id="rId1"/>
+    <sheet name="Observations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>S.no</t>
   </si>
@@ -75,13 +76,22 @@
   </si>
   <si>
     <t xml:space="preserve">Unable to verify coyni support gmail </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Element Name </t>
+  </si>
+  <si>
+    <t>Buy Tokens-Debit,Credit</t>
+  </si>
+  <si>
+    <t>its showing Buy Token instead of Buy Tokens in Debit,Credit Transaction details</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +103,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,10 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,19 +456,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AAA837C-7835-4140-B739-A4DF39BFDDFB}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="43" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,7 +488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -490,7 +508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -514,4 +532,62 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D76FE9-B3D5-A941-8484-510D9333813B}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45132</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified test methods of customer portal and modified the test scripts and test data
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/AutmationBlockers.xlsx
+++ b/Mobile/coyni_mobile/resources/AutmationBlockers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ideyalabs/Documents/24-July-2023_v3.0_Android/coyni-automation/Mobile/coyni_mobile/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5D5C4E-9E73-044C-8ED2-ACE994E7AC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31117F11-23E7-2344-A031-FE6444F4F826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{6789F843-B6C6-469F-91AB-D7541C9DA822}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>S.no</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>its showing Buy Token instead of Buy Tokens in Debit,Credit Transaction details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send / Request </t>
+  </si>
+  <si>
+    <t>Add Card to Reload</t>
+  </si>
+  <si>
+    <t>Debit,Credit card address is  not auto populating without existing card but addressed already saved</t>
+  </si>
+  <si>
+    <t>Address fields</t>
   </si>
 </sst>
 </file>
@@ -536,15 +548,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D76FE9-B3D5-A941-8484-510D9333813B}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="4" width="15.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="61.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -587,6 +601,26 @@
         <v>15</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45141</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified the Test Scripts for Customer portal
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/AutmationBlockers.xlsx
+++ b/Mobile/coyni_mobile/resources/AutmationBlockers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ideyalabs/Documents/24-July-2023_v3.0_Android/coyni-automation/Mobile/coyni_mobile/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ideyalabs/Documents/03-Aug-2023_v3.0_Android/coyni-automation/Mobile/coyni_mobile/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31117F11-23E7-2344-A031-FE6444F4F826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5A19B1-6B31-6C46-9E11-3F6A7586AD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{6789F843-B6C6-469F-91AB-D7541C9DA822}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>S.no</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>Address fields</t>
+  </si>
+  <si>
+    <t>Add Debit/Credit Cards</t>
+  </si>
+  <si>
+    <t>Trying to add the existing card,its refreshing the card fields, after entering the valid new card details, address is not auto populating</t>
+  </si>
+  <si>
+    <t>Billing Address</t>
   </si>
 </sst>
 </file>
@@ -469,7 +478,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -548,15 +557,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D76FE9-B3D5-A941-8484-510D9333813B}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.33203125" customWidth="1"/>
     <col min="6" max="6" width="61.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -621,6 +631,26 @@
         <v>18</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>